<commit_message>
get stats & get quantity
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\4 Тестирование\Heroes_battle_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2840A897-F6D4-40C4-A579-CF43D34974B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB24701B-3B2F-45E4-8038-0C6DFA5336AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="753" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="753" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Метаданные" sheetId="1" r:id="rId1"/>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B26:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
unit abilities (easy part)
+ little bit of the bugfix
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\4 Тестирование\Heroes_battle_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB24701B-3B2F-45E4-8038-0C6DFA5336AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5E3AED-4817-42D1-BC01-EC6B593C25BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="753" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="753" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Метаданные" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="265">
   <si>
     <t>Название листа</t>
   </si>
@@ -814,6 +814,21 @@
   </si>
   <si>
     <t>Тестовые юниты</t>
+  </si>
+  <si>
+    <t>Яростный манекен</t>
+  </si>
+  <si>
+    <t>Стойкий яростный манекен</t>
+  </si>
+  <si>
+    <t>Живое существо, Гнев манекена</t>
+  </si>
+  <si>
+    <t>Ослабляющий удар, Нежить</t>
+  </si>
+  <si>
+    <t>Манекен зомби</t>
   </si>
 </sst>
 </file>
@@ -1269,15 +1284,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="5" width="10" customWidth="1"/>
@@ -1404,6 +1419,174 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>262</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>262</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>263</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1418,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
colors + initiative visualisation
Заменил цвета на стабильные Красный+Синий.
Развернул визуализацию шкалы инициативы чтобы порядок на шкале был слева направо.
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\4 Тестирование\Heroes_battle_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22011D8B-C142-4B00-957B-0E0313615FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D9AE67-974C-4555-9F80-6A7892C5C27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="753" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1392,7 @@
         <v>100</v>
       </c>
       <c r="G2">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="H2">
         <v>5</v>

</xml_diff>